<commit_message>
Added spring meeting 2006 to keyword demo
git-svn-id: https://linked-open-data-essi.googlecode.com/svn/trunk@141 b0185bf4-efdb-b751-5fae-c403f5f989be
</commit_message>
<xml_diff>
--- a/resources/demos/keyword_usage_data/essi_keywords.xlsx
+++ b/resources/demos/keyword_usage_data/essi_keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20680" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="-680" yWindow="140" windowWidth="20680" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2168,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C1632"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A1405" workbookViewId="0">
+      <selection activeCell="B1406" sqref="B1406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>